<commit_message>
Updated downtime and XP
</commit_message>
<xml_diff>
--- a/A1 - Downtime Activities/Downtime Activity Calculations.xlsx
+++ b/A1 - Downtime Activities/Downtime Activity Calculations.xlsx
@@ -5,16 +5,17 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\zach.vosburgh\source\repos\NeverwinterNights\A1 - Downtime Activities\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\zachv\repos\NeverwinterNights\A1 - Downtime Activities\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{FA56EF3C-08E9-4232-964D-47DFEFEBEDBC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{092CD76F-B682-4B76-931C-D530127041D4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-23148" yWindow="6792" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{93034098-8959-4563-91C5-A0E61D1C199E}"/>
+    <workbookView xWindow="16354" yWindow="-5717" windowWidth="20777" windowHeight="13200" activeTab="2" xr2:uid="{93034098-8959-4563-91C5-A0E61D1C199E}"/>
   </bookViews>
   <sheets>
     <sheet name="Downtime GP per session Calcula" sheetId="1" r:id="rId1"/>
     <sheet name="Downtime Feats Worth" sheetId="2" r:id="rId2"/>
+    <sheet name="Crafting with monster parts" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -37,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="102">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="109">
   <si>
     <t>Level</t>
   </si>
@@ -343,6 +344,27 @@
   </si>
   <si>
     <t>Number of games</t>
+  </si>
+  <si>
+    <t>Monster CR</t>
+  </si>
+  <si>
+    <t>Harvest DC 1</t>
+  </si>
+  <si>
+    <t>Harvest DC 2</t>
+  </si>
+  <si>
+    <t>Harvest DC 3</t>
+  </si>
+  <si>
+    <t>Harvest 1 Worth</t>
+  </si>
+  <si>
+    <t>Harvest 2 Worth</t>
+  </si>
+  <si>
+    <t>Harvest 3 Worth</t>
   </si>
 </sst>
 </file>
@@ -374,7 +396,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="10">
+  <borders count="11">
     <border>
       <left/>
       <right/>
@@ -517,17 +539,24 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -543,6 +572,11 @@
     <xf numFmtId="16" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="16" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -880,37 +914,37 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EECABC18-317B-4861-972D-995D288AED56}">
   <dimension ref="A1:S29"/>
   <sheetViews>
-    <sheetView topLeftCell="B4" workbookViewId="0">
-      <selection activeCell="J26" sqref="J26"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="K21" sqref="K21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="16.73046875" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="16.73046875" customWidth="1"/>
+    <col min="1" max="1" width="16.77734375" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="16.77734375" customWidth="1"/>
     <col min="5" max="5" width="14.33203125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.265625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="10.19921875" bestFit="1" customWidth="1"/>
-    <col min="8" max="9" width="14.06640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.21875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.21875" bestFit="1" customWidth="1"/>
+    <col min="8" max="9" width="14.109375" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="15" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="15.59765625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="15.59765625" customWidth="1"/>
-    <col min="13" max="13" width="9.06640625" customWidth="1"/>
+    <col min="11" max="11" width="15.5546875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="15.5546875" customWidth="1"/>
+    <col min="13" max="13" width="9.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" x14ac:dyDescent="0.45">
-      <c r="E1" s="3" t="s">
+    <row r="1" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="E1" s="14" t="s">
         <v>15</v>
       </c>
-      <c r="F1" s="3"/>
-      <c r="G1" s="3"/>
-      <c r="H1" s="3"/>
-      <c r="I1" s="3"/>
-      <c r="J1" s="3"/>
-      <c r="K1" s="3"/>
-      <c r="L1" s="2"/>
-    </row>
-    <row r="2" spans="1:19" x14ac:dyDescent="0.45">
+      <c r="F1" s="14"/>
+      <c r="G1" s="14"/>
+      <c r="H1" s="14"/>
+      <c r="I1" s="14"/>
+      <c r="J1" s="14"/>
+      <c r="K1" s="14"/>
+      <c r="L1" s="1"/>
+    </row>
+    <row r="2" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>19</v>
       </c>
@@ -944,98 +978,98 @@
       <c r="K2" t="s">
         <v>10</v>
       </c>
-      <c r="L2" t="s">
+      <c r="L2" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="M2" t="s">
+      <c r="M2" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="N2" t="s">
+      <c r="N2" s="12" t="s">
         <v>1</v>
       </c>
-      <c r="O2" s="1" t="s">
+      <c r="O2" s="15" t="s">
         <v>2</v>
       </c>
-      <c r="P2" t="s">
+      <c r="P2" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="Q2" t="s">
+      <c r="Q2" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="R2" t="s">
+      <c r="R2" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="S2" t="s">
+      <c r="S2" s="6" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:19" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>20</v>
       </c>
-      <c r="B3" s="4"/>
+      <c r="B3" s="2"/>
       <c r="D3">
         <v>1</v>
       </c>
-      <c r="L3">
+      <c r="L3" s="7">
         <v>1</v>
       </c>
-      <c r="M3">
+      <c r="M3" s="4">
         <v>3</v>
       </c>
-      <c r="N3">
+      <c r="N3" s="4">
         <v>-4</v>
       </c>
-      <c r="O3">
+      <c r="O3" s="4">
         <v>1</v>
       </c>
-      <c r="P3">
+      <c r="P3" s="4">
         <v>2</v>
       </c>
-      <c r="Q3">
+      <c r="Q3" s="4">
         <v>3</v>
       </c>
-      <c r="R3">
+      <c r="R3" s="4">
         <v>4</v>
       </c>
-      <c r="S3">
+      <c r="S3" s="8">
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:19" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>16</v>
       </c>
       <c r="D4">
         <v>2</v>
       </c>
-      <c r="L4">
+      <c r="L4" s="7">
         <v>2</v>
       </c>
-      <c r="M4">
+      <c r="M4" s="4">
         <v>6</v>
       </c>
-      <c r="N4">
+      <c r="N4" s="4">
         <v>-8</v>
       </c>
-      <c r="O4">
+      <c r="O4" s="4">
         <v>2</v>
       </c>
-      <c r="P4">
+      <c r="P4" s="4">
         <v>4</v>
       </c>
-      <c r="Q4">
+      <c r="Q4" s="4">
         <v>6</v>
       </c>
-      <c r="R4">
+      <c r="R4" s="4">
         <v>8</v>
       </c>
-      <c r="S4">
+      <c r="S4" s="8">
         <v>12</v>
       </c>
     </row>
-    <row r="5" spans="1:19" x14ac:dyDescent="0.45">
-      <c r="B5" s="4" t="s">
+    <row r="5" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="B5" s="2" t="s">
         <v>24</v>
       </c>
       <c r="C5">
@@ -1044,71 +1078,71 @@
       <c r="D5">
         <v>3</v>
       </c>
-      <c r="L5">
+      <c r="L5" s="7">
         <v>3</v>
       </c>
-      <c r="M5">
+      <c r="M5" s="4">
         <v>12</v>
       </c>
-      <c r="N5">
+      <c r="N5" s="4">
         <v>-16</v>
       </c>
-      <c r="O5">
+      <c r="O5" s="4">
         <v>4</v>
       </c>
-      <c r="P5">
+      <c r="P5" s="4">
         <v>8</v>
       </c>
-      <c r="Q5">
-        <f>M5</f>
+      <c r="Q5" s="4">
+        <f t="shared" ref="Q5:Q22" si="0">M5</f>
         <v>12</v>
       </c>
-      <c r="R5">
+      <c r="R5" s="4">
         <v>16</v>
       </c>
-      <c r="S5">
-        <f>M5*2</f>
+      <c r="S5" s="8">
+        <f t="shared" ref="S5:S22" si="1">M5*2</f>
         <v>24</v>
       </c>
     </row>
-    <row r="6" spans="1:19" x14ac:dyDescent="0.45">
-      <c r="B6" s="4" t="s">
+    <row r="6" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="B6" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="C6" s="5">
+      <c r="C6" s="3">
         <v>1500</v>
       </c>
       <c r="D6">
         <v>4</v>
       </c>
-      <c r="L6">
+      <c r="L6" s="7">
         <v>4</v>
       </c>
-      <c r="M6">
+      <c r="M6" s="4">
         <v>25</v>
       </c>
-      <c r="N6">
+      <c r="N6" s="4">
         <v>-33</v>
       </c>
-      <c r="O6">
+      <c r="O6" s="4">
         <v>8</v>
       </c>
-      <c r="P6">
+      <c r="P6" s="4">
         <v>16</v>
       </c>
-      <c r="Q6">
-        <f>M6</f>
+      <c r="Q6" s="4">
+        <f t="shared" si="0"/>
         <v>25</v>
       </c>
-      <c r="R6">
+      <c r="R6" s="4">
         <v>30</v>
       </c>
-      <c r="S6">
-        <f>M6*2</f>
+      <c r="S6" s="8">
+        <f t="shared" si="1"/>
         <v>50</v>
       </c>
     </row>
-    <row r="7" spans="1:19" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>17</v>
       </c>
@@ -1118,279 +1152,279 @@
       <c r="E7">
         <v>30</v>
       </c>
-      <c r="L7">
+      <c r="L7" s="7">
         <v>5</v>
       </c>
-      <c r="M7">
+      <c r="M7" s="4">
         <v>50</v>
       </c>
-      <c r="N7">
+      <c r="N7" s="4">
         <v>-66</v>
       </c>
-      <c r="O7">
+      <c r="O7" s="4">
         <v>16</v>
       </c>
-      <c r="P7">
+      <c r="P7" s="4">
         <v>30</v>
       </c>
-      <c r="Q7">
-        <f>M7</f>
+      <c r="Q7" s="4">
+        <f t="shared" si="0"/>
         <v>50</v>
       </c>
-      <c r="R7">
+      <c r="R7" s="4">
         <v>65</v>
       </c>
-      <c r="S7">
-        <f>M7*2</f>
+      <c r="S7" s="8">
+        <f t="shared" si="1"/>
         <v>100</v>
       </c>
     </row>
-    <row r="8" spans="1:19" x14ac:dyDescent="0.45">
-      <c r="B8" s="4" t="s">
+    <row r="8" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="B8" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="C8" s="5">
+      <c r="C8" s="3">
         <v>3500</v>
       </c>
       <c r="D8">
         <v>6</v>
       </c>
-      <c r="L8">
+      <c r="L8" s="7">
         <v>6</v>
       </c>
-      <c r="M8">
+      <c r="M8" s="4">
         <v>70</v>
       </c>
-      <c r="N8">
+      <c r="N8" s="4">
         <v>-90</v>
       </c>
-      <c r="O8">
+      <c r="O8" s="4">
         <v>20</v>
       </c>
-      <c r="P8">
+      <c r="P8" s="4">
         <v>45</v>
       </c>
-      <c r="Q8">
-        <f>M8</f>
+      <c r="Q8" s="4">
+        <f t="shared" si="0"/>
         <v>70</v>
       </c>
-      <c r="R8">
+      <c r="R8" s="4">
         <v>100</v>
       </c>
-      <c r="S8">
-        <f>M8*2</f>
+      <c r="S8" s="8">
+        <f t="shared" si="1"/>
         <v>140</v>
       </c>
     </row>
-    <row r="9" spans="1:19" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:19" x14ac:dyDescent="0.3">
       <c r="D9">
         <v>7</v>
       </c>
-      <c r="L9">
+      <c r="L9" s="7">
         <v>7</v>
       </c>
-      <c r="M9">
+      <c r="M9" s="4">
         <v>90</v>
       </c>
-      <c r="N9">
+      <c r="N9" s="4">
         <v>-120</v>
       </c>
-      <c r="O9">
+      <c r="O9" s="4">
         <v>30</v>
       </c>
-      <c r="P9">
+      <c r="P9" s="4">
         <v>60</v>
       </c>
-      <c r="Q9">
-        <f>M9</f>
+      <c r="Q9" s="4">
+        <f t="shared" si="0"/>
         <v>90</v>
       </c>
-      <c r="R9">
+      <c r="R9" s="4">
         <v>120</v>
       </c>
-      <c r="S9">
-        <f>M9*2</f>
+      <c r="S9" s="8">
+        <f t="shared" si="1"/>
         <v>180</v>
       </c>
     </row>
-    <row r="10" spans="1:19" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:19" x14ac:dyDescent="0.3">
       <c r="D10">
         <v>8</v>
       </c>
-      <c r="L10">
+      <c r="L10" s="7">
         <v>8</v>
       </c>
-      <c r="M10">
+      <c r="M10" s="4">
         <v>120</v>
       </c>
-      <c r="N10">
+      <c r="N10" s="4">
         <v>-160</v>
       </c>
-      <c r="O10">
+      <c r="O10" s="4">
         <v>40</v>
       </c>
-      <c r="P10">
+      <c r="P10" s="4">
         <v>80</v>
       </c>
-      <c r="Q10">
-        <f>M10</f>
+      <c r="Q10" s="4">
+        <f t="shared" si="0"/>
         <v>120</v>
       </c>
-      <c r="R10">
+      <c r="R10" s="4">
         <v>160</v>
       </c>
-      <c r="S10">
-        <f>M10*2</f>
+      <c r="S10" s="8">
+        <f t="shared" si="1"/>
         <v>240</v>
       </c>
     </row>
-    <row r="11" spans="1:19" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:19" x14ac:dyDescent="0.3">
       <c r="D11">
         <v>9</v>
       </c>
       <c r="F11">
         <v>30</v>
       </c>
-      <c r="L11">
+      <c r="L11" s="7">
         <v>9</v>
       </c>
-      <c r="M11">
+      <c r="M11" s="4">
         <v>150</v>
       </c>
-      <c r="N11">
+      <c r="N11" s="4">
         <v>-200</v>
       </c>
-      <c r="O11">
+      <c r="O11" s="4">
         <v>50</v>
       </c>
-      <c r="P11">
+      <c r="P11" s="4">
         <v>100</v>
       </c>
-      <c r="Q11">
-        <f>M11</f>
+      <c r="Q11" s="4">
+        <f t="shared" si="0"/>
         <v>150</v>
       </c>
-      <c r="R11">
+      <c r="R11" s="4">
         <v>200</v>
       </c>
-      <c r="S11">
-        <f>M11*2</f>
+      <c r="S11" s="8">
+        <f t="shared" si="1"/>
         <v>300</v>
       </c>
     </row>
-    <row r="12" spans="1:19" x14ac:dyDescent="0.45">
-      <c r="B12" s="4" t="s">
+    <row r="12" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="B12" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="C12" s="5">
+      <c r="C12" s="3">
         <v>6400</v>
       </c>
       <c r="D12">
         <v>10</v>
       </c>
-      <c r="L12">
+      <c r="L12" s="7">
         <v>10</v>
       </c>
-      <c r="M12">
+      <c r="M12" s="4">
         <v>180</v>
       </c>
-      <c r="N12">
+      <c r="N12" s="4">
         <v>-240</v>
       </c>
-      <c r="O12">
+      <c r="O12" s="4">
         <v>60</v>
       </c>
-      <c r="P12">
+      <c r="P12" s="4">
         <v>120</v>
       </c>
-      <c r="Q12">
-        <f>M12</f>
+      <c r="Q12" s="4">
+        <f t="shared" si="0"/>
         <v>180</v>
       </c>
-      <c r="R12">
+      <c r="R12" s="4">
         <v>240</v>
       </c>
-      <c r="S12">
-        <f>M12*2</f>
+      <c r="S12" s="8">
+        <f t="shared" si="1"/>
         <v>360</v>
       </c>
     </row>
-    <row r="13" spans="1:19" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>18</v>
       </c>
       <c r="D13">
         <v>11</v>
       </c>
-      <c r="L13">
+      <c r="L13" s="7">
         <v>11</v>
       </c>
-      <c r="M13">
+      <c r="M13" s="4">
         <v>220</v>
       </c>
-      <c r="N13">
+      <c r="N13" s="4">
         <v>-295</v>
       </c>
-      <c r="O13">
+      <c r="O13" s="4">
         <v>70</v>
       </c>
-      <c r="P13">
+      <c r="P13" s="4">
         <v>150</v>
       </c>
-      <c r="Q13">
-        <f>M13</f>
+      <c r="Q13" s="4">
+        <f t="shared" si="0"/>
         <v>220</v>
       </c>
-      <c r="R13">
+      <c r="R13" s="4">
         <v>300</v>
       </c>
-      <c r="S13">
-        <f>M13*2</f>
+      <c r="S13" s="8">
+        <f t="shared" si="1"/>
         <v>440</v>
       </c>
     </row>
-    <row r="14" spans="1:19" x14ac:dyDescent="0.45">
-      <c r="B14" s="4" t="s">
+    <row r="14" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="B14" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="C14" s="5">
+      <c r="C14" s="3">
         <v>8030</v>
       </c>
       <c r="D14">
         <v>12</v>
       </c>
-      <c r="L14">
+      <c r="L14" s="7">
         <v>12</v>
       </c>
-      <c r="M14">
+      <c r="M14" s="4">
         <v>260</v>
       </c>
-      <c r="N14">
+      <c r="N14" s="4">
         <v>-350</v>
       </c>
-      <c r="O14">
+      <c r="O14" s="4">
         <v>85</v>
       </c>
-      <c r="P14">
+      <c r="P14" s="4">
         <v>175</v>
       </c>
-      <c r="Q14">
-        <f>M14</f>
+      <c r="Q14" s="4">
+        <f t="shared" si="0"/>
         <v>260</v>
       </c>
-      <c r="R14">
+      <c r="R14" s="4">
         <v>350</v>
       </c>
-      <c r="S14">
-        <f>M14*2</f>
+      <c r="S14" s="8">
+        <f t="shared" si="1"/>
         <v>520</v>
       </c>
     </row>
-    <row r="15" spans="1:19" x14ac:dyDescent="0.45">
-      <c r="B15" s="4" t="s">
+    <row r="15" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="B15" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="C15" s="5">
+      <c r="C15" s="3">
         <v>8030</v>
       </c>
       <c r="D15">
@@ -1399,112 +1433,112 @@
       <c r="G15">
         <v>30</v>
       </c>
-      <c r="L15">
+      <c r="L15" s="7">
         <v>13</v>
       </c>
-      <c r="M15">
+      <c r="M15" s="4">
         <v>300</v>
       </c>
-      <c r="N15">
+      <c r="N15" s="4">
         <v>-400</v>
       </c>
-      <c r="O15">
+      <c r="O15" s="4">
         <v>100</v>
       </c>
-      <c r="P15">
+      <c r="P15" s="4">
         <v>200</v>
       </c>
-      <c r="Q15">
-        <f>M15</f>
+      <c r="Q15" s="4">
+        <f t="shared" si="0"/>
         <v>300</v>
       </c>
-      <c r="R15">
+      <c r="R15" s="4">
         <v>400</v>
       </c>
-      <c r="S15">
-        <f>M15*2</f>
+      <c r="S15" s="8">
+        <f t="shared" si="1"/>
         <v>600</v>
       </c>
     </row>
-    <row r="16" spans="1:19" x14ac:dyDescent="0.45">
-      <c r="B16" s="4" t="s">
+    <row r="16" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="B16" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="C16" s="5">
+      <c r="C16" s="3">
         <v>12000</v>
       </c>
       <c r="D16">
         <v>14</v>
       </c>
-      <c r="L16">
+      <c r="L16" s="7">
         <v>14</v>
       </c>
-      <c r="M16">
+      <c r="M16" s="4">
         <v>400</v>
       </c>
-      <c r="N16">
+      <c r="N16" s="4">
         <v>-550</v>
       </c>
-      <c r="O16">
+      <c r="O16" s="4">
         <v>130</v>
       </c>
-      <c r="P16">
+      <c r="P16" s="4">
         <v>250</v>
       </c>
-      <c r="Q16">
-        <f>M16</f>
+      <c r="Q16" s="4">
+        <f t="shared" si="0"/>
         <v>400</v>
       </c>
-      <c r="R16">
+      <c r="R16" s="4">
         <v>550</v>
       </c>
-      <c r="S16">
-        <f>M16*2</f>
+      <c r="S16" s="8">
+        <f t="shared" si="1"/>
         <v>800</v>
       </c>
     </row>
-    <row r="17" spans="1:19" x14ac:dyDescent="0.45">
-      <c r="B17" s="4" t="s">
+    <row r="17" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="B17" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="C17" s="5">
+      <c r="C17" s="3">
         <v>16100</v>
       </c>
       <c r="D17">
         <v>15</v>
       </c>
-      <c r="L17">
+      <c r="L17" s="7">
         <v>15</v>
       </c>
-      <c r="M17">
+      <c r="M17" s="4">
         <v>500</v>
       </c>
-      <c r="N17">
+      <c r="N17" s="4">
         <v>-650</v>
       </c>
-      <c r="O17">
+      <c r="O17" s="4">
         <v>170</v>
       </c>
-      <c r="P17">
+      <c r="P17" s="4">
         <v>350</v>
       </c>
-      <c r="Q17">
-        <f>M17</f>
+      <c r="Q17" s="4">
+        <f t="shared" si="0"/>
         <v>500</v>
       </c>
-      <c r="R17">
+      <c r="R17" s="4">
         <v>650</v>
       </c>
-      <c r="S17">
-        <f>M17*2</f>
+      <c r="S17" s="8">
+        <f t="shared" si="1"/>
         <v>1000</v>
       </c>
     </row>
-    <row r="18" spans="1:19" x14ac:dyDescent="0.45">
-      <c r="B18" s="4" t="s">
+    <row r="18" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="B18" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="C18" s="5">
+      <c r="C18" s="3">
         <v>24000</v>
       </c>
       <c r="D18">
@@ -1513,78 +1547,78 @@
       <c r="H18">
         <v>30</v>
       </c>
-      <c r="L18">
+      <c r="L18" s="7">
         <v>16</v>
       </c>
-      <c r="M18">
+      <c r="M18" s="4">
         <v>600</v>
       </c>
-      <c r="N18">
+      <c r="N18" s="4">
         <v>-800</v>
       </c>
-      <c r="O18">
+      <c r="O18" s="4">
         <v>200</v>
       </c>
-      <c r="P18">
+      <c r="P18" s="4">
         <v>400</v>
       </c>
-      <c r="Q18">
-        <f>M18</f>
+      <c r="Q18" s="4">
+        <f t="shared" si="0"/>
         <v>600</v>
       </c>
-      <c r="R18">
+      <c r="R18" s="4">
         <v>800</v>
       </c>
-      <c r="S18">
-        <f>M18*2</f>
+      <c r="S18" s="8">
+        <f t="shared" si="1"/>
         <v>1200</v>
       </c>
     </row>
-    <row r="19" spans="1:19" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>14</v>
       </c>
-      <c r="B19" s="4" t="s">
+      <c r="B19" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="C19" s="5">
+      <c r="C19" s="3">
         <v>30000</v>
       </c>
       <c r="D19">
         <v>17</v>
       </c>
-      <c r="L19">
+      <c r="L19" s="7">
         <v>17</v>
       </c>
-      <c r="M19">
+      <c r="M19" s="4">
         <v>1000</v>
       </c>
-      <c r="N19">
+      <c r="N19" s="4">
         <v>-1300</v>
       </c>
-      <c r="O19">
+      <c r="O19" s="4">
         <v>350</v>
       </c>
-      <c r="P19">
+      <c r="P19" s="4">
         <v>650</v>
       </c>
-      <c r="Q19">
-        <f>M19</f>
+      <c r="Q19" s="4">
+        <f t="shared" si="0"/>
         <v>1000</v>
       </c>
-      <c r="R19">
+      <c r="R19" s="4">
         <v>1300</v>
       </c>
-      <c r="S19">
-        <f>M19*2</f>
+      <c r="S19" s="8">
+        <f t="shared" si="1"/>
         <v>2000</v>
       </c>
     </row>
-    <row r="20" spans="1:19" x14ac:dyDescent="0.45">
-      <c r="B20" s="4" t="s">
+    <row r="20" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="B20" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="C20" s="5">
+      <c r="C20" s="3">
         <v>32000</v>
       </c>
       <c r="D20">
@@ -1593,75 +1627,75 @@
       <c r="I20">
         <v>30</v>
       </c>
-      <c r="L20">
+      <c r="L20" s="7">
         <v>18</v>
       </c>
-      <c r="M20">
+      <c r="M20" s="4">
         <v>1500</v>
       </c>
-      <c r="N20">
+      <c r="N20" s="4">
         <v>-2000</v>
       </c>
-      <c r="O20">
+      <c r="O20" s="4">
         <v>500</v>
       </c>
-      <c r="P20">
+      <c r="P20" s="4">
         <v>1000</v>
       </c>
-      <c r="Q20">
-        <f>M20</f>
+      <c r="Q20" s="4">
+        <f t="shared" si="0"/>
         <v>1500</v>
       </c>
-      <c r="R20">
+      <c r="R20" s="4">
         <v>2000</v>
       </c>
-      <c r="S20">
-        <f>M20*2</f>
+      <c r="S20" s="8">
+        <f t="shared" si="1"/>
         <v>3000</v>
       </c>
     </row>
-    <row r="21" spans="1:19" x14ac:dyDescent="0.45">
-      <c r="B21" s="4" t="s">
+    <row r="21" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="B21" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="C21" s="5">
+      <c r="C21" s="3">
         <v>60000</v>
       </c>
       <c r="D21">
         <v>19</v>
       </c>
-      <c r="L21">
+      <c r="L21" s="7">
         <v>19</v>
       </c>
-      <c r="M21">
+      <c r="M21" s="4">
         <v>2250</v>
       </c>
-      <c r="N21">
+      <c r="N21" s="4">
         <v>-3000</v>
       </c>
-      <c r="O21">
+      <c r="O21" s="4">
         <v>750</v>
       </c>
-      <c r="P21">
+      <c r="P21" s="4">
         <v>1500</v>
       </c>
-      <c r="Q21">
-        <f>M21</f>
+      <c r="Q21" s="4">
+        <f t="shared" si="0"/>
         <v>2250</v>
       </c>
-      <c r="R21">
+      <c r="R21" s="4">
         <v>3000</v>
       </c>
-      <c r="S21">
-        <f>M21*2</f>
+      <c r="S21" s="8">
+        <f t="shared" si="1"/>
         <v>4500</v>
       </c>
     </row>
-    <row r="22" spans="1:19" x14ac:dyDescent="0.45">
+    <row r="22" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B22" t="s">
         <v>37</v>
       </c>
-      <c r="C22" s="5">
+      <c r="C22" s="3">
         <v>165000</v>
       </c>
       <c r="D22">
@@ -1670,49 +1704,49 @@
       <c r="J22">
         <v>30</v>
       </c>
-      <c r="L22">
+      <c r="L22" s="9">
         <v>20</v>
       </c>
-      <c r="M22">
+      <c r="M22" s="13">
         <v>3000</v>
       </c>
-      <c r="N22">
+      <c r="N22" s="13">
         <v>-4000</v>
       </c>
-      <c r="O22">
+      <c r="O22" s="13">
         <v>1000</v>
       </c>
-      <c r="P22">
+      <c r="P22" s="13">
         <v>2000</v>
       </c>
-      <c r="Q22">
-        <f>M22</f>
+      <c r="Q22" s="13">
+        <f t="shared" si="0"/>
         <v>3000</v>
       </c>
-      <c r="R22">
+      <c r="R22" s="13">
         <v>4000</v>
       </c>
-      <c r="S22">
-        <f>M22*2</f>
+      <c r="S22" s="10">
+        <f t="shared" si="1"/>
         <v>6000</v>
       </c>
     </row>
-    <row r="23" spans="1:19" x14ac:dyDescent="0.45">
+    <row r="23" spans="1:19" x14ac:dyDescent="0.3">
       <c r="B23" t="s">
         <v>36</v>
       </c>
-      <c r="C23" s="5">
+      <c r="C23" s="3">
         <v>318000</v>
       </c>
     </row>
-    <row r="26" spans="1:19" x14ac:dyDescent="0.45">
-      <c r="G26" s="3" t="s">
+    <row r="26" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="G26" s="14" t="s">
         <v>96</v>
       </c>
-      <c r="H26" s="3"/>
-      <c r="I26" s="3"/>
-    </row>
-    <row r="27" spans="1:19" x14ac:dyDescent="0.45">
+      <c r="H26" s="14"/>
+      <c r="I26" s="14"/>
+    </row>
+    <row r="27" spans="1:19" x14ac:dyDescent="0.3">
       <c r="F27" t="s">
         <v>97</v>
       </c>
@@ -1729,7 +1763,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="28" spans="1:19" x14ac:dyDescent="0.45">
+    <row r="28" spans="1:19" x14ac:dyDescent="0.3">
       <c r="F28">
         <v>8</v>
       </c>
@@ -1748,7 +1782,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="29" spans="1:19" x14ac:dyDescent="0.45">
+    <row r="29" spans="1:19" x14ac:dyDescent="0.3">
       <c r="F29">
         <v>8</v>
       </c>
@@ -1795,19 +1829,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C86A2C11-BE8A-439F-9527-E84F63BC50CF}">
   <dimension ref="A1:P22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="J16" sqref="J16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="17.86328125" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="11.9296875" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="8.59765625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="17.88671875" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="11.88671875" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="8.5546875" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="22.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>38</v>
       </c>
@@ -1832,21 +1866,21 @@
       <c r="H1" t="s">
         <v>39</v>
       </c>
-      <c r="K1" s="7" t="s">
+      <c r="K1" s="5" t="s">
         <v>41</v>
       </c>
-      <c r="L1" s="8"/>
-      <c r="N1" s="7" t="s">
+      <c r="L1" s="6"/>
+      <c r="N1" s="5" t="s">
         <v>53</v>
       </c>
-      <c r="O1" s="14" t="s">
+      <c r="O1" s="12" t="s">
         <v>54</v>
       </c>
-      <c r="P1" s="8" t="s">
+      <c r="P1" s="6" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>74</v>
       </c>
@@ -1863,7 +1897,7 @@
         <v>0</v>
       </c>
       <c r="F2">
-        <f>SUM(B2:E2)</f>
+        <f t="shared" ref="F2:F9" si="0">SUM(B2:E2)</f>
         <v>39</v>
       </c>
       <c r="G2" t="s">
@@ -1873,21 +1907,21 @@
         <f>F2*1.2*100</f>
         <v>4680</v>
       </c>
-      <c r="K2" s="9" t="s">
+      <c r="K2" s="7" t="s">
         <v>42</v>
       </c>
-      <c r="L2" s="10" t="s">
+      <c r="L2" s="8" t="s">
         <v>47</v>
       </c>
-      <c r="N2" s="9" t="s">
+      <c r="N2" s="7" t="s">
         <v>55</v>
       </c>
-      <c r="O2" s="6" t="s">
+      <c r="O2" s="4" t="s">
         <v>62</v>
       </c>
-      <c r="P2" s="10"/>
-    </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.45">
+      <c r="P2" s="8"/>
+    </row>
+    <row r="3" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>40</v>
       </c>
@@ -1904,33 +1938,33 @@
         <v>0</v>
       </c>
       <c r="F3">
-        <f>SUM(B3:E3)</f>
+        <f t="shared" si="0"/>
         <v>62</v>
       </c>
       <c r="G3" t="s">
         <v>42</v>
       </c>
       <c r="H3">
-        <f t="shared" ref="H3:H22" si="0">F3*1.2*100</f>
+        <f t="shared" ref="H3:H22" si="1">F3*1.2*100</f>
         <v>7439.9999999999991</v>
       </c>
-      <c r="K3" s="9" t="s">
+      <c r="K3" s="7" t="s">
         <v>43</v>
       </c>
-      <c r="L3" s="10" t="s">
+      <c r="L3" s="8" t="s">
         <v>48</v>
       </c>
-      <c r="N3" s="9" t="s">
+      <c r="N3" s="7" t="s">
         <v>56</v>
       </c>
-      <c r="O3" s="13" t="s">
+      <c r="O3" s="11" t="s">
         <v>60</v>
       </c>
-      <c r="P3" s="10" t="s">
+      <c r="P3" s="8" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="4" spans="1:16" ht="28.25" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:16" ht="28.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>75</v>
       </c>
@@ -1947,33 +1981,33 @@
         <v>8</v>
       </c>
       <c r="F4">
-        <f>SUM(B4:E4)</f>
+        <f t="shared" si="0"/>
         <v>43</v>
       </c>
       <c r="G4" t="s">
         <v>44</v>
       </c>
       <c r="H4">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>5160</v>
       </c>
-      <c r="K4" s="9" t="s">
+      <c r="K4" s="7" t="s">
         <v>44</v>
       </c>
-      <c r="L4" s="10" t="s">
+      <c r="L4" s="8" t="s">
         <v>49</v>
       </c>
-      <c r="N4" s="9" t="s">
+      <c r="N4" s="7" t="s">
         <v>59</v>
       </c>
-      <c r="O4" s="6" t="s">
+      <c r="O4" s="4" t="s">
         <v>61</v>
       </c>
-      <c r="P4" s="10" t="s">
+      <c r="P4" s="8" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>76</v>
       </c>
@@ -1984,33 +2018,33 @@
         <v>10</v>
       </c>
       <c r="F5">
-        <f>SUM(B5:E5)</f>
+        <f t="shared" si="0"/>
         <v>20</v>
       </c>
       <c r="G5" t="s">
         <v>77</v>
       </c>
       <c r="H5">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>2400</v>
       </c>
-      <c r="K5" s="9" t="s">
+      <c r="K5" s="7" t="s">
         <v>45</v>
       </c>
-      <c r="L5" s="10" t="s">
+      <c r="L5" s="8" t="s">
         <v>50</v>
       </c>
-      <c r="N5" s="9" t="s">
+      <c r="N5" s="7" t="s">
         <v>64</v>
       </c>
-      <c r="O5" s="6" t="s">
+      <c r="O5" s="4" t="s">
         <v>65</v>
       </c>
-      <c r="P5" s="10" t="s">
+      <c r="P5" s="8" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="6" spans="1:16" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="6" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>78</v>
       </c>
@@ -2024,33 +2058,33 @@
         <v>50</v>
       </c>
       <c r="F6">
-        <f>SUM(B6:E6)</f>
+        <f t="shared" si="0"/>
         <v>80</v>
       </c>
       <c r="G6" t="s">
         <v>42</v>
       </c>
       <c r="H6">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>9600</v>
       </c>
-      <c r="K6" s="9" t="s">
+      <c r="K6" s="7" t="s">
         <v>46</v>
       </c>
-      <c r="L6" s="10" t="s">
+      <c r="L6" s="8" t="s">
         <v>51</v>
       </c>
-      <c r="N6" s="11" t="s">
+      <c r="N6" s="9" t="s">
         <v>67</v>
       </c>
-      <c r="O6" s="15" t="s">
+      <c r="O6" s="13" t="s">
         <v>68</v>
       </c>
-      <c r="P6" s="12" t="s">
+      <c r="P6" s="10" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="7" spans="1:16" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="7" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>80</v>
       </c>
@@ -2058,24 +2092,24 @@
         <v>37</v>
       </c>
       <c r="F7">
-        <f>SUM(B7:E7)</f>
+        <f t="shared" si="0"/>
         <v>37</v>
       </c>
       <c r="G7" t="s">
         <v>46</v>
       </c>
       <c r="H7">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>4440</v>
       </c>
-      <c r="K7" s="11" t="s">
+      <c r="K7" s="9" t="s">
         <v>77</v>
       </c>
-      <c r="L7" s="12" t="s">
+      <c r="L7" s="10" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>81</v>
       </c>
@@ -2089,18 +2123,18 @@
         <v>10</v>
       </c>
       <c r="F8">
-        <f>SUM(B8:E8)</f>
+        <f t="shared" si="0"/>
         <v>40</v>
       </c>
       <c r="G8" t="s">
         <v>45</v>
       </c>
       <c r="H8">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>4800</v>
       </c>
     </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>82</v>
       </c>
@@ -2117,18 +2151,18 @@
         <v>5</v>
       </c>
       <c r="F9">
-        <f>SUM(B9:E9)</f>
+        <f t="shared" si="0"/>
         <v>19</v>
       </c>
       <c r="G9" t="s">
         <v>77</v>
       </c>
       <c r="H9">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>2280</v>
       </c>
     </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>83</v>
       </c>
@@ -2139,18 +2173,18 @@
         <v>15</v>
       </c>
       <c r="F10">
-        <f t="shared" ref="F10:F22" si="1">SUM(B10:E10)</f>
+        <f t="shared" ref="F10:F22" si="2">SUM(B10:E10)</f>
         <v>35</v>
       </c>
       <c r="G10" t="s">
         <v>46</v>
       </c>
       <c r="H10">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>4200</v>
       </c>
     </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>84</v>
       </c>
@@ -2161,18 +2195,18 @@
         <v>6</v>
       </c>
       <c r="F11">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>31</v>
       </c>
       <c r="G11" t="s">
         <v>77</v>
       </c>
       <c r="H11">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>3719.9999999999995</v>
       </c>
     </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>85</v>
       </c>
@@ -2183,18 +2217,18 @@
         <v>10</v>
       </c>
       <c r="F12">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>20</v>
       </c>
       <c r="G12" t="s">
         <v>77</v>
       </c>
       <c r="H12">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>2400</v>
       </c>
     </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>86</v>
       </c>
@@ -2205,18 +2239,18 @@
         <v>40</v>
       </c>
       <c r="F13">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>63</v>
       </c>
       <c r="G13" t="s">
         <v>42</v>
       </c>
       <c r="H13">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>7559.9999999999991</v>
       </c>
     </row>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>87</v>
       </c>
@@ -2227,18 +2261,18 @@
         <v>25</v>
       </c>
       <c r="F14">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>50</v>
       </c>
       <c r="G14" t="s">
         <v>43</v>
       </c>
       <c r="H14">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>6000</v>
       </c>
     </row>
-    <row r="15" spans="1:16" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>88</v>
       </c>
@@ -2249,18 +2283,18 @@
         <v>15</v>
       </c>
       <c r="F15">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>35</v>
       </c>
       <c r="G15" t="s">
         <v>46</v>
       </c>
       <c r="H15">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>4200</v>
       </c>
     </row>
-    <row r="16" spans="1:16" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>89</v>
       </c>
@@ -2271,18 +2305,18 @@
         <v>25</v>
       </c>
       <c r="F16">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>45</v>
       </c>
       <c r="G16" t="s">
         <v>44</v>
       </c>
       <c r="H16">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>5400</v>
       </c>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>90</v>
       </c>
@@ -2290,18 +2324,18 @@
         <v>48</v>
       </c>
       <c r="F17">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>48</v>
       </c>
       <c r="G17" t="s">
         <v>44</v>
       </c>
       <c r="H17">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>5759.9999999999991</v>
       </c>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>91</v>
       </c>
@@ -2318,18 +2352,18 @@
         <v>15</v>
       </c>
       <c r="F18">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>39</v>
       </c>
       <c r="G18" t="s">
         <v>45</v>
       </c>
       <c r="H18">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>4680</v>
       </c>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>92</v>
       </c>
@@ -2340,18 +2374,18 @@
         <v>10</v>
       </c>
       <c r="F19">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>32</v>
       </c>
       <c r="G19" t="s">
         <v>77</v>
       </c>
       <c r="H19">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>3840</v>
       </c>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>93</v>
       </c>
@@ -2365,18 +2399,18 @@
         <v>3</v>
       </c>
       <c r="F20">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>26</v>
       </c>
       <c r="G20" t="s">
         <v>77</v>
       </c>
       <c r="H20">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>3120</v>
       </c>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>94</v>
       </c>
@@ -2387,18 +2421,18 @@
         <v>35</v>
       </c>
       <c r="F21">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>70</v>
       </c>
       <c r="G21" t="s">
         <v>42</v>
       </c>
       <c r="H21">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>8400</v>
       </c>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>95</v>
       </c>
@@ -2412,15 +2446,484 @@
         <v>13</v>
       </c>
       <c r="F22">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>38</v>
       </c>
       <c r="G22" t="s">
         <v>45</v>
       </c>
       <c r="H22">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>4560</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DA1182D9-9F77-427D-AB6D-CD8D0E6BD41F}">
+  <dimension ref="A1:H26"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E2" sqref="E2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="10.5546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="11.77734375" bestFit="1" customWidth="1"/>
+    <col min="5" max="7" width="14.33203125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>102</v>
+      </c>
+      <c r="B1" t="s">
+        <v>103</v>
+      </c>
+      <c r="C1" t="s">
+        <v>104</v>
+      </c>
+      <c r="D1" t="s">
+        <v>105</v>
+      </c>
+      <c r="E1" t="s">
+        <v>106</v>
+      </c>
+      <c r="F1" t="s">
+        <v>107</v>
+      </c>
+      <c r="G1" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A2">
+        <v>2</v>
+      </c>
+      <c r="B2">
+        <v>6</v>
+      </c>
+      <c r="C2">
+        <v>9</v>
+      </c>
+      <c r="D2">
+        <v>11</v>
+      </c>
+      <c r="H2" s="4">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A3">
+        <v>3</v>
+      </c>
+      <c r="B3">
+        <v>6</v>
+      </c>
+      <c r="C3">
+        <v>9</v>
+      </c>
+      <c r="D3">
+        <v>11</v>
+      </c>
+      <c r="H3" s="4">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A4">
+        <v>4</v>
+      </c>
+      <c r="B4">
+        <v>6</v>
+      </c>
+      <c r="C4">
+        <v>9</v>
+      </c>
+      <c r="D4">
+        <v>11</v>
+      </c>
+      <c r="H4" s="4">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A5">
+        <v>5</v>
+      </c>
+      <c r="B5">
+        <v>8</v>
+      </c>
+      <c r="C5">
+        <v>11</v>
+      </c>
+      <c r="D5">
+        <v>13</v>
+      </c>
+      <c r="H5" s="4">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A6">
+        <v>6</v>
+      </c>
+      <c r="B6">
+        <v>8</v>
+      </c>
+      <c r="C6">
+        <v>11</v>
+      </c>
+      <c r="D6">
+        <v>13</v>
+      </c>
+      <c r="H6" s="4">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A7">
+        <v>7</v>
+      </c>
+      <c r="B7">
+        <v>8</v>
+      </c>
+      <c r="C7">
+        <v>11</v>
+      </c>
+      <c r="D7">
+        <v>13</v>
+      </c>
+      <c r="H7" s="4">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A8">
+        <v>8</v>
+      </c>
+      <c r="B8">
+        <v>10</v>
+      </c>
+      <c r="C8">
+        <v>13</v>
+      </c>
+      <c r="D8">
+        <v>15</v>
+      </c>
+      <c r="H8" s="4">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A9">
+        <v>9</v>
+      </c>
+      <c r="B9">
+        <v>10</v>
+      </c>
+      <c r="C9">
+        <v>13</v>
+      </c>
+      <c r="D9">
+        <v>15</v>
+      </c>
+      <c r="H9" s="4">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A10">
+        <v>10</v>
+      </c>
+      <c r="B10">
+        <v>10</v>
+      </c>
+      <c r="C10">
+        <v>13</v>
+      </c>
+      <c r="D10">
+        <v>15</v>
+      </c>
+      <c r="H10" s="4">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A11">
+        <v>11</v>
+      </c>
+      <c r="B11">
+        <v>12</v>
+      </c>
+      <c r="C11">
+        <v>15</v>
+      </c>
+      <c r="D11">
+        <v>17</v>
+      </c>
+      <c r="H11" s="4">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A12">
+        <v>12</v>
+      </c>
+      <c r="B12">
+        <v>12</v>
+      </c>
+      <c r="C12">
+        <v>15</v>
+      </c>
+      <c r="D12">
+        <v>17</v>
+      </c>
+      <c r="H12" s="4">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A13">
+        <v>13</v>
+      </c>
+      <c r="B13">
+        <v>12</v>
+      </c>
+      <c r="C13">
+        <v>15</v>
+      </c>
+      <c r="D13">
+        <v>17</v>
+      </c>
+      <c r="H13" s="4">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A14">
+        <v>14</v>
+      </c>
+      <c r="B14">
+        <v>14</v>
+      </c>
+      <c r="C14">
+        <v>17</v>
+      </c>
+      <c r="D14">
+        <v>19</v>
+      </c>
+      <c r="H14" s="4">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A15">
+        <v>15</v>
+      </c>
+      <c r="B15">
+        <v>14</v>
+      </c>
+      <c r="C15">
+        <v>17</v>
+      </c>
+      <c r="D15">
+        <v>19</v>
+      </c>
+      <c r="H15" s="4">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A16">
+        <v>16</v>
+      </c>
+      <c r="B16">
+        <v>14</v>
+      </c>
+      <c r="C16">
+        <v>17</v>
+      </c>
+      <c r="D16">
+        <v>19</v>
+      </c>
+      <c r="H16" s="4">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A17">
+        <v>17</v>
+      </c>
+      <c r="B17">
+        <v>16</v>
+      </c>
+      <c r="C17">
+        <v>19</v>
+      </c>
+      <c r="D17">
+        <v>21</v>
+      </c>
+      <c r="H17" s="4">
+        <v>600</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A18">
+        <v>18</v>
+      </c>
+      <c r="B18">
+        <v>16</v>
+      </c>
+      <c r="C18">
+        <v>19</v>
+      </c>
+      <c r="D18">
+        <v>21</v>
+      </c>
+      <c r="H18" s="4">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A19">
+        <v>19</v>
+      </c>
+      <c r="B19">
+        <v>16</v>
+      </c>
+      <c r="C19">
+        <v>19</v>
+      </c>
+      <c r="D19">
+        <v>21</v>
+      </c>
+      <c r="H19" s="4">
+        <v>1500</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A20">
+        <v>20</v>
+      </c>
+      <c r="B20">
+        <v>18</v>
+      </c>
+      <c r="C20">
+        <v>21</v>
+      </c>
+      <c r="D20">
+        <v>23</v>
+      </c>
+      <c r="H20" s="4">
+        <v>2250</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A21">
+        <v>21</v>
+      </c>
+      <c r="B21">
+        <v>18</v>
+      </c>
+      <c r="C21">
+        <v>21</v>
+      </c>
+      <c r="D21">
+        <v>23</v>
+      </c>
+      <c r="H21" s="13">
+        <v>3000</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A22">
+        <v>22</v>
+      </c>
+      <c r="B22">
+        <v>18</v>
+      </c>
+      <c r="C22">
+        <v>21</v>
+      </c>
+      <c r="D22">
+        <v>23</v>
+      </c>
+      <c r="H22" s="16">
+        <v>3500</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A23">
+        <v>23</v>
+      </c>
+      <c r="B23">
+        <v>18</v>
+      </c>
+      <c r="C23">
+        <v>21</v>
+      </c>
+      <c r="D23">
+        <v>23</v>
+      </c>
+      <c r="H23" s="16">
+        <v>4000</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A24">
+        <v>24</v>
+      </c>
+      <c r="B24">
+        <v>20</v>
+      </c>
+      <c r="C24">
+        <v>23</v>
+      </c>
+      <c r="D24">
+        <v>25</v>
+      </c>
+      <c r="H24" s="16">
+        <v>4500</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A25">
+        <v>25</v>
+      </c>
+      <c r="B25">
+        <v>20</v>
+      </c>
+      <c r="C25">
+        <v>23</v>
+      </c>
+      <c r="D25">
+        <v>25</v>
+      </c>
+      <c r="H25" s="16">
+        <v>5000</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A26">
+        <v>26</v>
+      </c>
+      <c r="B26">
+        <v>20</v>
+      </c>
+      <c r="C26">
+        <v>23</v>
+      </c>
+      <c r="D26">
+        <v>25</v>
+      </c>
+      <c r="H26" s="16">
+        <v>5500</v>
       </c>
     </row>
   </sheetData>

</xml_diff>